<commit_message>
Updated payment and checkout pages
</commit_message>
<xml_diff>
--- a/orders.xlsx
+++ b/orders.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R7"/>
+  <dimension ref="A1:S8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -524,6 +524,11 @@
           <t>Delivery</t>
         </is>
       </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Payment Screenshot</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -576,6 +581,7 @@
       <c r="P2" t="inlineStr"/>
       <c r="Q2" t="inlineStr"/>
       <c r="R2" t="inlineStr"/>
+      <c r="S2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
@@ -624,6 +630,7 @@
       </c>
       <c r="Q3" t="inlineStr"/>
       <c r="R3" t="inlineStr"/>
+      <c r="S3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr"/>
@@ -676,6 +683,7 @@
       <c r="R4" t="n">
         <v>59</v>
       </c>
+      <c r="S4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr"/>
@@ -728,6 +736,7 @@
       <c r="R5" t="n">
         <v>59</v>
       </c>
+      <c r="S5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr"/>
@@ -780,6 +789,7 @@
       <c r="R6" t="n">
         <v>59</v>
       </c>
+      <c r="S6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr"/>
@@ -798,10 +808,8 @@
           <t xml:space="preserve">jeevan </t>
         </is>
       </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>121004</t>
-        </is>
+      <c r="I7" t="n">
+        <v>121004</v>
       </c>
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
@@ -833,6 +841,66 @@
       </c>
       <c r="R7" t="n">
         <v>59</v>
+      </c>
+      <c r="S7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr"/>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>12345678978</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>jeevan</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>121004</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>ORD20250731165620</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>pratibha</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>Light Green Dress (₹250 x 1), Mala Set of 8 (₹240 x 1)</t>
+        </is>
+      </c>
+      <c r="O8" t="n">
+        <v>549</v>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>2025-07-31 16:56</t>
+        </is>
+      </c>
+      <c r="Q8" t="n">
+        <v>490</v>
+      </c>
+      <c r="R8" t="n">
+        <v>59</v>
+      </c>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>static/payments/ORD20250731165620.jpeg</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>